<commit_message>
0.3 ops.. pushed old files, these are the proper files for 0.3a
</commit_message>
<xml_diff>
--- a/Perceptron Todo.xlsx
+++ b/Perceptron Todo.xlsx
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -242,17 +242,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -291,6 +280,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,12 +292,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,6 +306,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -631,7 +620,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,27 +645,27 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,26 +749,26 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="7">
         <v>42392</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -788,10 +777,10 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="7">
         <v>42392</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
@@ -802,10 +791,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="7">
         <v>42392</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -814,10 +803,10 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="7">
         <v>42392</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -826,10 +815,10 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>42392</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -838,10 +827,10 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="7">
         <v>42392</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -850,10 +839,10 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="7">
         <v>42392</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -864,10 +853,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="7">
         <v>42392</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -876,25 +865,25 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>

</xml_diff>

<commit_message>
0.4a Prep work for multi layered nn
-Create a class hierarchy for neural nets
-Add back propagation for sigmoid function
-Add momentum and weight decay
</commit_message>
<xml_diff>
--- a/Perceptron Todo.xlsx
+++ b/Perceptron Todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -95,6 +95,39 @@
   </si>
   <si>
     <t>Create an automated test to remove columns that reduce the effectiveness of the system</t>
+  </si>
+  <si>
+    <t>Create a class hirachy for neural nets</t>
+  </si>
+  <si>
+    <t>This will let me keep my old school pcn around</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0.4a</t>
+  </si>
+  <si>
+    <t>Create a tool to measure convergance speed</t>
+  </si>
+  <si>
+    <t>In iterations</t>
+  </si>
+  <si>
+    <t>Create a '1 layered' PCM with back propigation</t>
+  </si>
+  <si>
+    <t>Add momentum and weight decay</t>
+  </si>
+  <si>
+    <t>Prep work for Multi Layered NN</t>
+  </si>
+  <si>
+    <t>0.5a</t>
+  </si>
+  <si>
+    <t>Multi Layered NN</t>
   </si>
 </sst>
 </file>
@@ -283,6 +316,21 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,23 +340,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -617,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,27 +678,27 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,26 +782,26 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>42392</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -780,7 +813,7 @@
       <c r="A15" s="7">
         <v>42392</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
@@ -794,7 +827,7 @@
       <c r="A16" s="7">
         <v>42392</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -806,7 +839,7 @@
       <c r="A17" s="7">
         <v>42392</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -818,7 +851,7 @@
       <c r="A18" s="7">
         <v>42392</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -830,7 +863,7 @@
       <c r="A19" s="7">
         <v>42392</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -842,7 +875,7 @@
       <c r="A20" s="7">
         <v>42392</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -856,7 +889,7 @@
       <c r="A21" s="7">
         <v>42392</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -865,31 +898,113 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="7">
+        <v>42393</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="7">
+        <v>42393</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>42393</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:C13"/>

</xml_diff>

<commit_message>
0.5a Two layered NN
</commit_message>
<xml_diff>
--- a/Perceptron Todo.xlsx
+++ b/Perceptron Todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Create a tool to measure convergance speed</t>
   </si>
   <si>
-    <t>In iterations</t>
-  </si>
-  <si>
     <t>Create a '1 layered' PCM with back propigation</t>
   </si>
   <si>
@@ -128,6 +125,12 @@
   </si>
   <si>
     <t>Multi Layered NN</t>
+  </si>
+  <si>
+    <t>Create a two layered neural net</t>
+  </si>
+  <si>
+    <t>Needed some help from example code for this, forgot to threshold the hidden layer…</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +910,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -935,7 +938,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -947,13 +950,13 @@
         <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="1"/>
@@ -961,30 +964,36 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="7">
+        <v>42393</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
0.6a Three Layer Neural Net
-Use 1/sqrt(n) for initial weights
-Add over fitting testing to training
-Randomised input order
-Create three layered nerual net
</commit_message>
<xml_diff>
--- a/Perceptron Todo.xlsx
+++ b/Perceptron Todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,60 @@
   </si>
   <si>
     <t>Needed some help from example code for this, forgot to threshold the hidden layer…</t>
+  </si>
+  <si>
+    <t>Use 1/sqrt(n) for initial weights</t>
+  </si>
+  <si>
+    <t>Dual Layered NN</t>
+  </si>
+  <si>
+    <t>0.6a</t>
+  </si>
+  <si>
+    <t>drop1 error testing</t>
+  </si>
+  <si>
+    <t>Create three layered nerual net</t>
+  </si>
+  <si>
+    <t>Create mutli layered neural net</t>
+  </si>
+  <si>
+    <t>Where number of nodes at each layer can be specified</t>
+  </si>
+  <si>
+    <t>Allow nerual nets to be created with random properties</t>
+  </si>
+  <si>
+    <t>Number of layers etc</t>
+  </si>
+  <si>
+    <t>Create a survival game to find machines with good characteristics</t>
+  </si>
+  <si>
+    <t>See if we can get a score of 20 or less :)</t>
+  </si>
+  <si>
+    <t>Add over fitting testing to training</t>
+  </si>
+  <si>
+    <t>Randomised input order</t>
+  </si>
+  <si>
+    <t>Apparently helps with convergence speed, should test this</t>
+  </si>
+  <si>
+    <t>Three Layered NN</t>
+  </si>
+  <si>
+    <t>0.7a</t>
+  </si>
+  <si>
+    <t>0.8a</t>
+  </si>
+  <si>
+    <t>Fitness Algorithm</t>
   </si>
 </sst>
 </file>
@@ -653,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +1018,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
@@ -985,33 +1039,201 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>42394</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>42394</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>42394</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>42394</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:C28"/>
+  <mergeCells count="15">
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A2:C2"/>
@@ -1019,6 +1241,14 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>